<commit_message>
Test data for performance
Test data for performance
</commit_message>
<xml_diff>
--- a/CapellaUI/resources/TestData.xlsx
+++ b/CapellaUI/resources/TestData.xlsx
@@ -8,18 +8,20 @@
   </bookViews>
   <sheets>
     <sheet name="CurrentLabsTest" sheetId="6" r:id="rId1"/>
-    <sheet name="MedicalEquipmentTest" sheetId="8" r:id="rId2"/>
-    <sheet name="PerformanceTest" sheetId="9" r:id="rId3"/>
-    <sheet name="ProvidersTeamTest" sheetId="10" r:id="rId4"/>
-    <sheet name="ReferralsTest" sheetId="11" r:id="rId5"/>
-    <sheet name="UnitTest" sheetId="2" r:id="rId6"/>
+    <sheet name="ManageDocumentsTest" sheetId="12" r:id="rId2"/>
+    <sheet name="MaterialFulfillmentTest" sheetId="13" r:id="rId3"/>
+    <sheet name="MedicalEquipmentTest" sheetId="8" r:id="rId4"/>
+    <sheet name="PerformanceTest" sheetId="9" r:id="rId5"/>
+    <sheet name="ProvidersTeamTest" sheetId="10" r:id="rId6"/>
+    <sheet name="ReferralsTest" sheetId="11" r:id="rId7"/>
+    <sheet name="UnitTest" sheetId="2" r:id="rId8"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="322" uniqueCount="127">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="448" uniqueCount="172">
   <si>
     <t>paige</t>
   </si>
@@ -400,13 +402,148 @@
   </si>
   <si>
     <t>TONY</t>
+  </si>
+  <si>
+    <t>EMAIL</t>
+  </si>
+  <si>
+    <t>ADDRESS</t>
+  </si>
+  <si>
+    <t>APTSUITE</t>
+  </si>
+  <si>
+    <t>CITY</t>
+  </si>
+  <si>
+    <t>STATE</t>
+  </si>
+  <si>
+    <t>ZIP</t>
+  </si>
+  <si>
+    <t>yo.dude@villagehealth.com</t>
+  </si>
+  <si>
+    <t>3 W Hawthorn Parkway</t>
+  </si>
+  <si>
+    <t>Vernon Hills</t>
+  </si>
+  <si>
+    <t>DOCUMENTDESCRITION</t>
+  </si>
+  <si>
+    <t>DOCUMENTTYPEOPTION</t>
+  </si>
+  <si>
+    <t>verify_AddingaDocument</t>
+  </si>
+  <si>
+    <t>Emelita Coulahan</t>
+  </si>
+  <si>
+    <t>Verify add document automation</t>
+  </si>
+  <si>
+    <t>Diabetic Retinal Eye Exam Verification</t>
+  </si>
+  <si>
+    <t>MATERIAL</t>
+  </si>
+  <si>
+    <t>DATEREQUESTED</t>
+  </si>
+  <si>
+    <t>REQUESTEDBY</t>
+  </si>
+  <si>
+    <t>FOLLOWUP</t>
+  </si>
+  <si>
+    <t>ORDERTYPE</t>
+  </si>
+  <si>
+    <t>FULFILLEDBY</t>
+  </si>
+  <si>
+    <t>FULFILLEDON</t>
+  </si>
+  <si>
+    <t>verify_OrderingMaterial</t>
+  </si>
+  <si>
+    <t>Aasaf Whoriskey</t>
+  </si>
+  <si>
+    <t>Cholesterol Facts(Spanish)</t>
+  </si>
+  <si>
+    <t>TANYA COOK</t>
+  </si>
+  <si>
+    <t>In Person</t>
+  </si>
+  <si>
+    <t>Fitness &amp; Heart Disease</t>
+  </si>
+  <si>
+    <t>Mail Order</t>
+  </si>
+  <si>
+    <t>PHONE</t>
+  </si>
+  <si>
+    <t>FAX</t>
+  </si>
+  <si>
+    <t>OTHERPHONE</t>
+  </si>
+  <si>
+    <t>ALLOWCOMMUNICATION</t>
+  </si>
+  <si>
+    <t>FAXNUMBERVERIFIED</t>
+  </si>
+  <si>
+    <t>PATIENTSEEINGSINCE</t>
+  </si>
+  <si>
+    <t>ASSOCIATEAS</t>
+  </si>
+  <si>
+    <t>Illinois</t>
+  </si>
+  <si>
+    <t>(847) 123-1234</t>
+  </si>
+  <si>
+    <t>(847) 123-1235</t>
+  </si>
+  <si>
+    <t>(847) 123-1236</t>
+  </si>
+  <si>
+    <t>8/4/2017</t>
+  </si>
+  <si>
+    <t>verify_AddingProvider</t>
+  </si>
+  <si>
+    <t>DAVITA DELTONA DIALYSIS</t>
+  </si>
+  <si>
+    <t>PCP</t>
+  </si>
+  <si>
+    <t>TINA ALLEN</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -433,6 +570,13 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color rgb="FF333333"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -473,7 +617,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -511,6 +655,14 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -521,6 +673,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -815,9 +970,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AE7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I1" sqref="I1"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1484,8 +1637,238 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I5"/>
   <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="30.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.140625" customWidth="1"/>
+    <col min="5" max="5" width="31" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="35.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="17.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>136</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="H1" s="5" t="s">
+        <v>91</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="3"/>
+      <c r="B2" s="4" t="s">
+        <v>138</v>
+      </c>
+      <c r="C2" s="14" t="s">
+        <v>139</v>
+      </c>
+      <c r="D2" s="3">
+        <v>-1</v>
+      </c>
+      <c r="E2" s="6" t="s">
+        <v>140</v>
+      </c>
+      <c r="F2" s="6" t="s">
+        <v>141</v>
+      </c>
+      <c r="G2" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="H2" s="6" t="s">
+        <v>97</v>
+      </c>
+      <c r="I2" s="6" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" s="3"/>
+      <c r="B3" s="4"/>
+      <c r="C3" s="3"/>
+      <c r="D3" s="3"/>
+      <c r="E3" s="6"/>
+      <c r="F3" s="6"/>
+      <c r="G3" s="6"/>
+      <c r="H3" s="6"/>
+      <c r="I3" s="6"/>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" s="3"/>
+      <c r="B4" s="4"/>
+      <c r="C4" s="3"/>
+      <c r="D4" s="3"/>
+      <c r="E4" s="6"/>
+      <c r="F4" s="6"/>
+      <c r="G4" s="6"/>
+      <c r="H4" s="6"/>
+      <c r="I4" s="6"/>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5" s="3"/>
+      <c r="B5" s="4"/>
+      <c r="C5" s="3"/>
+      <c r="D5" s="3"/>
+      <c r="E5" s="6"/>
+      <c r="F5" s="6"/>
+      <c r="G5" s="6"/>
+      <c r="H5" s="6"/>
+      <c r="I5" s="6"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:J3"/>
+  <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+      <selection activeCell="E3" sqref="A1:J3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.28515625" style="3" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="24.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16" style="3" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.28515625" style="3" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.5703125" style="3" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.7109375" style="3" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>149</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>150</v>
+      </c>
+      <c r="D2" t="s">
+        <v>151</v>
+      </c>
+      <c r="E2" s="3">
+        <v>-3</v>
+      </c>
+      <c r="F2" t="s">
+        <v>152</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="H2" s="3" t="s">
+        <v>153</v>
+      </c>
+      <c r="I2" s="3" t="s">
+        <v>152</v>
+      </c>
+      <c r="J2" s="3">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>149</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>150</v>
+      </c>
+      <c r="D3" t="s">
+        <v>154</v>
+      </c>
+      <c r="E3" s="3">
+        <v>0</v>
+      </c>
+      <c r="F3" t="s">
+        <v>152</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="H3" s="3" t="s">
+        <v>155</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:I5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1644,19 +2027,19 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AK11"/>
+  <dimension ref="A1:AR11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="L2" sqref="L2"/>
+    <sheetView tabSelected="1" topLeftCell="AB1" workbookViewId="0">
+      <selection activeCell="AL3" sqref="AL3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="18.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.85546875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="5.5703125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="20.5703125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="19.5703125" bestFit="1" customWidth="1"/>
@@ -1691,9 +2074,16 @@
     <col min="35" max="35" width="5.28515625" bestFit="1" customWidth="1"/>
     <col min="36" max="36" width="24.5703125" bestFit="1" customWidth="1"/>
     <col min="37" max="37" width="25.7109375" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="24.85546875" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="16" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="41" max="41" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="42" max="42" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="43" max="43" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="44" max="44" width="12.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:37" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:44" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>53</v>
       </c>
@@ -1805,8 +2195,29 @@
       <c r="AK1" s="5" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="2" spans="1:37" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="AL1" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="AM1" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="AN1" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="AO1" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="AP1" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="AQ1" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="AR1" s="2" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="2" spans="1:44" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>14</v>
       </c>
@@ -1912,8 +2323,29 @@
       <c r="AK2" s="6">
         <v>30</v>
       </c>
-    </row>
-    <row r="3" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="AL2" t="s">
+        <v>151</v>
+      </c>
+      <c r="AM2" s="3">
+        <v>-3</v>
+      </c>
+      <c r="AN2" t="s">
+        <v>171</v>
+      </c>
+      <c r="AO2" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="AP2" s="3" t="s">
+        <v>153</v>
+      </c>
+      <c r="AQ2" t="s">
+        <v>171</v>
+      </c>
+      <c r="AR2" s="3">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>12</v>
       </c>
@@ -2019,8 +2451,25 @@
       <c r="AK3" s="6">
         <v>30</v>
       </c>
-    </row>
-    <row r="4" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="AL3" t="s">
+        <v>154</v>
+      </c>
+      <c r="AM3" s="3">
+        <v>0</v>
+      </c>
+      <c r="AN3" t="s">
+        <v>171</v>
+      </c>
+      <c r="AO3" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="AP3" s="3" t="s">
+        <v>155</v>
+      </c>
+      <c r="AQ3" s="3"/>
+      <c r="AR3" s="3"/>
+    </row>
+    <row r="4" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>14</v>
       </c>
@@ -2126,8 +2575,29 @@
       <c r="AK4" s="6">
         <v>30</v>
       </c>
-    </row>
-    <row r="5" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="AL4" t="s">
+        <v>151</v>
+      </c>
+      <c r="AM4" s="3">
+        <v>-3</v>
+      </c>
+      <c r="AN4" t="s">
+        <v>171</v>
+      </c>
+      <c r="AO4" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="AP4" s="3" t="s">
+        <v>153</v>
+      </c>
+      <c r="AQ4" t="s">
+        <v>171</v>
+      </c>
+      <c r="AR4" s="3">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>12</v>
       </c>
@@ -2233,8 +2703,25 @@
       <c r="AK5" s="6">
         <v>30</v>
       </c>
-    </row>
-    <row r="6" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="AL5" t="s">
+        <v>154</v>
+      </c>
+      <c r="AM5" s="3">
+        <v>0</v>
+      </c>
+      <c r="AN5" t="s">
+        <v>171</v>
+      </c>
+      <c r="AO5" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="AP5" s="3" t="s">
+        <v>155</v>
+      </c>
+      <c r="AQ5" s="3"/>
+      <c r="AR5" s="3"/>
+    </row>
+    <row r="6" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>14</v>
       </c>
@@ -2340,8 +2827,29 @@
       <c r="AK6" s="6">
         <v>30</v>
       </c>
-    </row>
-    <row r="7" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="AL6" t="s">
+        <v>151</v>
+      </c>
+      <c r="AM6" s="3">
+        <v>-3</v>
+      </c>
+      <c r="AN6" t="s">
+        <v>171</v>
+      </c>
+      <c r="AO6" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="AP6" s="3" t="s">
+        <v>153</v>
+      </c>
+      <c r="AQ6" t="s">
+        <v>171</v>
+      </c>
+      <c r="AR6" s="3">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>12</v>
       </c>
@@ -2447,8 +2955,25 @@
       <c r="AK7" s="6">
         <v>30</v>
       </c>
-    </row>
-    <row r="8" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="AL7" t="s">
+        <v>154</v>
+      </c>
+      <c r="AM7" s="3">
+        <v>0</v>
+      </c>
+      <c r="AN7" t="s">
+        <v>171</v>
+      </c>
+      <c r="AO7" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="AP7" s="3" t="s">
+        <v>155</v>
+      </c>
+      <c r="AQ7" s="3"/>
+      <c r="AR7" s="3"/>
+    </row>
+    <row r="8" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>14</v>
       </c>
@@ -2554,8 +3079,29 @@
       <c r="AK8" s="6">
         <v>30</v>
       </c>
-    </row>
-    <row r="9" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="AL8" t="s">
+        <v>151</v>
+      </c>
+      <c r="AM8" s="3">
+        <v>-3</v>
+      </c>
+      <c r="AN8" t="s">
+        <v>171</v>
+      </c>
+      <c r="AO8" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="AP8" s="3" t="s">
+        <v>153</v>
+      </c>
+      <c r="AQ8" t="s">
+        <v>171</v>
+      </c>
+      <c r="AR8" s="3">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>14</v>
       </c>
@@ -2661,8 +3207,25 @@
       <c r="AK9" s="6">
         <v>30</v>
       </c>
-    </row>
-    <row r="10" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="AL9" t="s">
+        <v>154</v>
+      </c>
+      <c r="AM9" s="3">
+        <v>0</v>
+      </c>
+      <c r="AN9" t="s">
+        <v>171</v>
+      </c>
+      <c r="AO9" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="AP9" s="3" t="s">
+        <v>155</v>
+      </c>
+      <c r="AQ9" s="3"/>
+      <c r="AR9" s="3"/>
+    </row>
+    <row r="10" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>14</v>
       </c>
@@ -2768,8 +3331,29 @@
       <c r="AK10" s="6">
         <v>30</v>
       </c>
-    </row>
-    <row r="11" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="AL10" t="s">
+        <v>151</v>
+      </c>
+      <c r="AM10" s="3">
+        <v>-3</v>
+      </c>
+      <c r="AN10" t="s">
+        <v>171</v>
+      </c>
+      <c r="AO10" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="AP10" s="3" t="s">
+        <v>153</v>
+      </c>
+      <c r="AQ10" t="s">
+        <v>171</v>
+      </c>
+      <c r="AR10" s="3">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>14</v>
       </c>
@@ -2875,6 +3459,23 @@
       <c r="AK11" s="6">
         <v>30</v>
       </c>
+      <c r="AL11" t="s">
+        <v>154</v>
+      </c>
+      <c r="AM11" s="3">
+        <v>0</v>
+      </c>
+      <c r="AN11" t="s">
+        <v>171</v>
+      </c>
+      <c r="AO11" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="AP11" s="3" t="s">
+        <v>155</v>
+      </c>
+      <c r="AQ11" s="3"/>
+      <c r="AR11" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2882,13 +3483,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:S4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -2897,9 +3496,15 @@
     <col min="3" max="3" width="17.7109375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="10.42578125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="8.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="26.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="21.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="6.28515625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="6" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>53</v>
       </c>
@@ -2915,11 +3520,51 @@
       <c r="E1" s="2" t="s">
         <v>117</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
-        <v>12</v>
-      </c>
+      <c r="F1" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>156</v>
+      </c>
+      <c r="M1" s="2" t="s">
+        <v>157</v>
+      </c>
+      <c r="N1" s="2" t="s">
+        <v>158</v>
+      </c>
+      <c r="O1" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="P1" s="2" t="s">
+        <v>160</v>
+      </c>
+      <c r="Q1" s="2" t="s">
+        <v>161</v>
+      </c>
+      <c r="R1" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="S1" s="2" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="2" spans="1:19" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="3"/>
       <c r="B2" s="3" t="s">
         <v>118</v>
       </c>
@@ -2932,17 +3577,109 @@
       <c r="E2" s="3" t="s">
         <v>120</v>
       </c>
+      <c r="F2" s="13" t="s">
+        <v>133</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>134</v>
+      </c>
+      <c r="H2" s="3">
+        <v>209</v>
+      </c>
+      <c r="I2" s="3" t="s">
+        <v>135</v>
+      </c>
+      <c r="J2" s="3" t="s">
+        <v>163</v>
+      </c>
+      <c r="K2" s="3">
+        <v>60061</v>
+      </c>
+      <c r="L2" s="3" t="s">
+        <v>164</v>
+      </c>
+      <c r="M2" s="3" t="s">
+        <v>165</v>
+      </c>
+      <c r="N2" s="3" t="s">
+        <v>166</v>
+      </c>
+      <c r="O2" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="P2" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="Q2" s="15" t="s">
+        <v>167</v>
+      </c>
+      <c r="S2" s="3"/>
+    </row>
+    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A3" s="3"/>
+      <c r="B3" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>119</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>120</v>
+      </c>
+      <c r="F3" s="13" t="s">
+        <v>133</v>
+      </c>
+      <c r="G3" s="3"/>
+      <c r="H3" s="3"/>
+      <c r="I3" s="3"/>
+      <c r="J3" s="3"/>
+      <c r="K3" s="3"/>
+      <c r="Q3" s="16"/>
+      <c r="S3" s="3"/>
+    </row>
+    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>168</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>150</v>
+      </c>
+      <c r="D4" s="3"/>
+      <c r="E4" s="3"/>
+      <c r="F4" s="3"/>
+      <c r="G4" s="3"/>
+      <c r="H4" s="3"/>
+      <c r="I4" s="3"/>
+      <c r="J4" s="3"/>
+      <c r="K4" s="3"/>
+      <c r="Q4" s="16"/>
+      <c r="R4" t="s">
+        <v>169</v>
+      </c>
+      <c r="S4" s="3" t="s">
+        <v>170</v>
+      </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="F2" r:id="rId1"/>
+    <hyperlink ref="F3" r:id="rId2"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
@@ -2994,7 +3731,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P7"/>
   <sheetViews>

</xml_diff>